<commit_message>
too-map fix spinal nerve root region location
</commit_message>
<xml_diff>
--- a/models/too-map/source/too-map.xlsx
+++ b/models/too-map/source/too-map.xlsx
@@ -1324,7 +1324,7 @@
     <t>Infracervical Autonomic Ganglia</t>
   </si>
   <si>
-    <t>{"x": -60, "y": 5},{"x": -60, "y": 15},{"x": -5, "y": 15},{"x": -5, "y": 5}</t>
+    <t>{"x": -60, "y": 17},{"x": -60, "y": 22},{"x": -5, "y": 22},{"x": -5, "y": 17}</t>
   </si>
   <si>
     <t>FMA:6475, FMA:6476, FMA:6477, FMA:6478, FMA:6479, FMA:6480, FMA:6481, FMA:6482, FMA:6483, FMA:6484, FMA:6485, ILX:0739295, FMA:6545, FMA:6541, FMA:6542, FMA:6543, ILX:0739296, ILX:0739297, FMA:6552, FMA:6559, FMA:6554, FMA:6555, FMA:6556, FMA:6783</t>
@@ -1947,7 +1947,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2157,6 +2157,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -5974,7 +5977,7 @@
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="64" t="s">
+      <c r="F21" s="74" t="s">
         <v>434</v>
       </c>
       <c r="G21" s="60" t="s">
@@ -5988,7 +5991,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="75" t="s">
         <v>437</v>
       </c>
       <c r="B22" s="68" t="s">
@@ -5999,7 +6002,7 @@
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="75" t="s">
+      <c r="F22" s="76" t="s">
         <v>439</v>
       </c>
       <c r="G22" s="60" t="s">
@@ -6082,7 +6085,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="76" t="s">
+      <c r="A26" s="77" t="s">
         <v>455</v>
       </c>
       <c r="B26" s="64" t="s">
@@ -6105,16 +6108,16 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="78" t="s">
         <v>460</v>
       </c>
-      <c r="B27" s="75" t="s">
+      <c r="B27" s="76" t="s">
         <v>461</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
-      <c r="F27" s="75" t="s">
+      <c r="F27" s="76" t="s">
         <v>462</v>
       </c>
       <c r="G27" s="71" t="s">
@@ -6128,7 +6131,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="77" t="s">
         <v>465</v>
       </c>
       <c r="B28" s="64" t="s">
@@ -6151,7 +6154,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="76" t="s">
+      <c r="A29" s="77" t="s">
         <v>470</v>
       </c>
       <c r="B29" s="64" t="s">
@@ -6206,7 +6209,7 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="78" t="s">
+      <c r="F31" s="79" t="s">
         <v>482</v>
       </c>
       <c r="G31" s="71" t="s">
@@ -6229,7 +6232,7 @@
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="78" t="s">
+      <c r="F32" s="79" t="s">
         <v>487</v>
       </c>
       <c r="G32" s="71" t="s">
@@ -6252,7 +6255,7 @@
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="78" t="s">
+      <c r="F33" s="79" t="s">
         <v>492</v>
       </c>
       <c r="G33" s="71" t="s">
@@ -6275,7 +6278,7 @@
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
-      <c r="F34" s="78" t="s">
+      <c r="F34" s="79" t="s">
         <v>497</v>
       </c>
       <c r="G34" s="71" t="s">
@@ -6298,7 +6301,7 @@
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
-      <c r="F35" s="78" t="s">
+      <c r="F35" s="79" t="s">
         <v>502</v>
       </c>
       <c r="G35" s="71" t="s">
@@ -6321,7 +6324,7 @@
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="F36" s="78" t="s">
+      <c r="F36" s="79" t="s">
         <v>507</v>
       </c>
       <c r="G36" s="71" t="s">
@@ -6344,7 +6347,7 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="78" t="s">
+      <c r="F37" s="79" t="s">
         <v>512</v>
       </c>
       <c r="G37" s="71" t="s">
@@ -6367,7 +6370,7 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="78" t="s">
+      <c r="F38" s="79" t="s">
         <v>517</v>
       </c>
       <c r="G38" s="71" t="s">
@@ -6390,7 +6393,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="F39" s="78" t="s">
+      <c r="F39" s="79" t="s">
         <v>522</v>
       </c>
       <c r="G39" s="71" t="s">
@@ -6413,7 +6416,7 @@
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
-      <c r="F40" s="78" t="s">
+      <c r="F40" s="79" t="s">
         <v>527</v>
       </c>
       <c r="G40" s="71" t="s">
@@ -6436,7 +6439,7 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="78" t="s">
+      <c r="F41" s="79" t="s">
         <v>532</v>
       </c>
       <c r="G41" s="71" t="s">
@@ -6459,7 +6462,7 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
-      <c r="F42" s="78" t="s">
+      <c r="F42" s="79" t="s">
         <v>537</v>
       </c>
       <c r="G42" s="71" t="s">
@@ -6522,8 +6525,8 @@
       <c r="C2" s="40" t="s">
         <v>545</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3">
       <c r="A3" s="38" t="s">
@@ -6535,8 +6538,8 @@
       <c r="C3" s="40" t="s">
         <v>548</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
     </row>
     <row r="4">
       <c r="A4" s="38" t="s">
@@ -6548,8 +6551,8 @@
       <c r="C4" s="40" t="s">
         <v>551</v>
       </c>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
     </row>
     <row r="5">
       <c r="A5" s="38" t="s">
@@ -6558,11 +6561,11 @@
       <c r="B5" s="38" t="s">
         <v>553</v>
       </c>
-      <c r="C5" s="79"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="40" t="s">
         <v>554</v>
       </c>
-      <c r="E5" s="79"/>
+      <c r="E5" s="80"/>
     </row>
     <row r="6">
       <c r="A6" s="38" t="s">
@@ -6571,11 +6574,11 @@
       <c r="B6" s="38" t="s">
         <v>556</v>
       </c>
-      <c r="C6" s="79"/>
+      <c r="C6" s="80"/>
       <c r="D6" s="40" t="s">
         <v>557</v>
       </c>
-      <c r="E6" s="79"/>
+      <c r="E6" s="80"/>
     </row>
     <row r="7">
       <c r="A7" s="38" t="s">
@@ -6584,11 +6587,11 @@
       <c r="B7" s="38" t="s">
         <v>559</v>
       </c>
-      <c r="C7" s="79"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="40" t="s">
         <v>560</v>
       </c>
-      <c r="E7" s="79"/>
+      <c r="E7" s="80"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
@@ -6597,8 +6600,8 @@
       <c r="B8" s="14" t="s">
         <v>562</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
       <c r="E8" s="40" t="s">
         <v>563</v>
       </c>
@@ -6610,7 +6613,7 @@
       <c r="B9" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="C9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="39"/>
       <c r="E9" s="47" t="s">
         <v>566</v>
@@ -6623,22 +6626,22 @@
       <c r="B10" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
       <c r="E10" s="40" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="81" t="s">
         <v>570</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="81" t="s">
         <v>571</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="81" t="s">
+      <c r="E11" s="82" t="s">
         <v>572</v>
       </c>
     </row>
@@ -6669,98 +6672,98 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="83" t="s">
         <v>574</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="84" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="83" t="s">
         <v>576</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="84" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="83" t="s">
         <v>578</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="84" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="83" t="s">
         <v>580</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="84" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="83" t="s">
         <v>582</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="84" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="83" t="s">
         <v>584</v>
       </c>
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="84" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="83" t="s">
         <v>586</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="84" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="83" t="s">
         <v>588</v>
       </c>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="84" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="83" t="s">
         <v>590</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="84" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="83" t="s">
         <v>592</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="84" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="83" t="s">
         <v>594</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="84" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="83" t="s">
         <v>596</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="84" t="s">
         <v>597</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to latest version from sheets
</commit_message>
<xml_diff>
--- a/models/too-map/source/too-map.xlsx
+++ b/models/too-map/source/too-map.xlsx
@@ -1303,7 +1303,7 @@
     <t>Pterygopalatine Ganglion, Submandibular Ganglion, Geniculate Ganglion, Nodose Ganglion, Petrous Ganglion, Jugular Ganglion, Superior Glossopharengeal Ganglion, Superior Cervical Ganglion, Middle Cervical Ganglion, Inferior Cervical Ganglion, Stellate Ganglion, Ciliary Ganglion, Trigeminal Ganglion, Otic Ganglion, T1 Sympathetic Ganglion, Vestibular Ganglion</t>
   </si>
   <si>
-    <t>n1N</t>
+    <t>n2N</t>
   </si>
   <si>
     <t>Infracranial Nerves</t>
@@ -1729,7 +1729,7 @@
     <t>N regions</t>
   </si>
   <si>
-    <t>n1,n2,n3,n4,n1H,n1T,n1P,n1A,n1G,n1N,n2G,n2R,n3A,n3M,n3L,n3U,n4c,n4V,n4R,n4O,n4C1N,n4C2N,n4C3N,n4C4N,n4C5N,n4C6N,n4C7N,n4C8N,n1C9N,n1C10N,n1C11N,n1C12N</t>
+    <t>n1,n2,n3,n4,n1H,n1T,n1P,n1A,n1G,n2N,n2G,n2R,n3A,n3M,n3L,n3U,n4c,n4V,n4R,n4O,n4C1N,n4C2N,n4C3N,n4C4N,n4C5N,n4C6N,n4C7N,n4C8N,n1C9N,n1C10N,n1C11N,n1C12N</t>
   </si>
   <si>
     <t>nerves</t>
@@ -1823,11 +1823,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1841,6 +1842,11 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color rgb="FF067D17"/>
@@ -1981,20 +1987,20 @@
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2006,28 +2012,28 @@
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2042,7 +2048,7 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2054,40 +2060,40 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -2097,20 +2103,20 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2137,10 +2143,10 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2155,28 +2161,28 @@
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2185,8 +2191,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2421,10 +2427,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="12.29"/>
-    <col customWidth="1" min="6" max="6" width="26.86"/>
+    <col customWidth="1" min="3" max="3" width="10.75"/>
+    <col customWidth="1" min="6" max="6" width="23.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2481,10 +2487,10 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="49.43"/>
-    <col customWidth="1" min="5" max="5" width="16.0"/>
+    <col customWidth="1" min="2" max="2" width="43.25"/>
+    <col customWidth="1" min="5" max="5" width="14.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3420,22 +3426,22 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.29"/>
-    <col customWidth="1" min="2" max="2" width="25.29"/>
-    <col customWidth="1" min="3" max="3" width="7.14"/>
-    <col customWidth="1" min="4" max="4" width="6.43"/>
-    <col customWidth="1" min="5" max="5" width="9.71"/>
-    <col customWidth="1" min="6" max="6" width="10.0"/>
-    <col customWidth="1" min="7" max="7" width="15.86"/>
-    <col customWidth="1" min="8" max="8" width="9.29"/>
-    <col customWidth="1" min="9" max="9" width="7.14"/>
-    <col customWidth="1" min="10" max="11" width="12.14"/>
-    <col customWidth="1" min="12" max="12" width="7.43"/>
-    <col customWidth="1" min="13" max="13" width="49.71"/>
-    <col customWidth="1" min="14" max="14" width="52.0"/>
-    <col customWidth="1" min="15" max="15" width="16.71"/>
+    <col customWidth="1" min="1" max="1" width="16.0"/>
+    <col customWidth="1" min="2" max="2" width="22.13"/>
+    <col customWidth="1" min="3" max="3" width="6.25"/>
+    <col customWidth="1" min="4" max="4" width="5.63"/>
+    <col customWidth="1" min="5" max="5" width="8.5"/>
+    <col customWidth="1" min="6" max="6" width="8.75"/>
+    <col customWidth="1" min="7" max="7" width="13.88"/>
+    <col customWidth="1" min="8" max="8" width="8.13"/>
+    <col customWidth="1" min="9" max="9" width="6.25"/>
+    <col customWidth="1" min="10" max="11" width="10.63"/>
+    <col customWidth="1" min="12" max="12" width="6.5"/>
+    <col customWidth="1" min="13" max="13" width="43.5"/>
+    <col customWidth="1" min="14" max="14" width="45.5"/>
+    <col customWidth="1" min="15" max="15" width="14.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5522,13 +5528,13 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="27.0"/>
-    <col customWidth="1" min="5" max="5" width="18.14"/>
-    <col customWidth="1" min="6" max="6" width="53.86"/>
-    <col customWidth="1" min="8" max="8" width="33.14"/>
-    <col customWidth="1" min="9" max="9" width="42.29"/>
+    <col customWidth="1" min="2" max="2" width="23.63"/>
+    <col customWidth="1" min="5" max="5" width="15.88"/>
+    <col customWidth="1" min="6" max="6" width="47.13"/>
+    <col customWidth="1" min="8" max="8" width="29.0"/>
+    <col customWidth="1" min="9" max="9" width="37.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6491,11 +6497,11 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="69.71"/>
-    <col customWidth="1" min="4" max="4" width="71.0"/>
-    <col customWidth="1" min="5" max="5" width="46.0"/>
+    <col customWidth="1" min="3" max="3" width="61.0"/>
+    <col customWidth="1" min="4" max="4" width="62.13"/>
+    <col customWidth="1" min="5" max="5" width="40.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6658,9 +6664,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="35.57"/>
+    <col customWidth="1" min="2" max="2" width="31.13"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Removed wrong references from "regions'
</commit_message>
<xml_diff>
--- a/models/too-map/source/too-map.xlsx
+++ b/models/too-map/source/too-map.xlsx
@@ -1743,7 +1743,7 @@
     <t>F wires</t>
   </si>
   <si>
-    <t>w-F,w-B-Z,w-Z-f1S,w-Z-X,w-X-f4E,w-X-f1L,w-X-O,w-B-O,w-O-f1P,w-O-f2L,w-O-R,w-R-G,w-G-f3G,w-G-U,w-U-f3K,w-U-M,w-R-M,w-M-f3M,w-M-W,w-W-f4C,w-W-J,w-J-f4P,w-J-V,w-V-f4N,w-f4N-f4P,w-f4P-f4L,w-f4N-f4E,w-V-f4N-f4E-X,w-f4E-f4M,w-V-B,w-M-B,w-F-B,w-F-O,w-F-R,w-F-M</t>
+    <t>w-F,w-B-Z,w-Z-f1S,w-Z-X,w-X-f4E,w-X-f1L,w-X-O,w-B-O,w-O-I, w-I-f1P,w-I-f2L,w-O-R,w-R-G,w-G-f3G,w-G-U,w-U-f3K,w-U-M,w-R-M,w-M-f3M,w-M-W,w-W-f4C,w-W-J,w-J-f4P,w-J-V,w-V-f4N,w-f4N-f4P,w-f4P-f4L,w-f4N-f4E,w-V-f4N-f4E-X,w-f4E-f4M,w-V-B,w-M-B,w-F-B,w-F-O,w-F-R,w-F-M</t>
   </si>
   <si>
     <t>wires-d</t>
@@ -1794,7 +1794,7 @@
     <t>nerves</t>
   </si>
   <si>
-    <t>Nerve regions</t>
+    <t>Cranial nerve regions</t>
   </si>
   <si>
     <t>n4C1N,n4C2N,n4C3N,n4C4N,n4C5N,n4C6N,n4C7N,n4C8N,n1C9N,n1C10N,n1C11N,n1C12N</t>
@@ -6750,7 +6750,7 @@
       <c r="A11" s="81" t="s">
         <v>577</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="3" t="s">
         <v>578</v>
       </c>
       <c r="C11" s="6"/>

</xml_diff>